<commit_message>
Fixed color alignment to profile. Added fifth color profile for ionic. Added accommodation for semicolon delimited data from HF IQ Chargers.
</commit_message>
<xml_diff>
--- a/Batterylocations.xlsx
+++ b/Batterylocations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgutierrez.MYSMITHFIELD\PycharmProjects\Chargerdataprocessor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7AC981-A0B9-4801-8552-CD0A79DF21EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7235725C-222A-47DA-A218-2EB7C02EB1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16140" yWindow="-4560" windowWidth="14400" windowHeight="10920" xr2:uid="{5F318202-7931-4863-97A9-CC32D701A797}"/>
+    <workbookView xWindow="-19590" yWindow="-1710" windowWidth="14100" windowHeight="10710" xr2:uid="{5F318202-7931-4863-97A9-CC32D701A797}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
   <si>
     <t>Location</t>
   </si>
@@ -172,6 +172,21 @@
   </si>
   <si>
     <t>Enersys mods</t>
+  </si>
+  <si>
+    <t>ML195059</t>
+  </si>
+  <si>
+    <t>Oldie</t>
+  </si>
+  <si>
+    <t>MJ190517</t>
+  </si>
+  <si>
+    <t>Boot Exchange</t>
+  </si>
+  <si>
+    <t>RTE 1</t>
   </si>
 </sst>
 </file>
@@ -530,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE12825-5FA0-48A1-B0CB-3F43941314C4}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,8 +816,31 @@
         <v>12</v>
       </c>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a few more instances to battery locations.
</commit_message>
<xml_diff>
--- a/Batterylocations.xlsx
+++ b/Batterylocations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgutierrez.MYSMITHFIELD\PycharmProjects\Chargerdataprocessor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7235725C-222A-47DA-A218-2EB7C02EB1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A294822-30CE-49E5-ACE4-3DD19B72B6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19590" yWindow="-1710" windowWidth="14100" windowHeight="10710" xr2:uid="{5F318202-7931-4863-97A9-CC32D701A797}"/>
+    <workbookView xWindow="-22440" yWindow="-330" windowWidth="14100" windowHeight="10710" xr2:uid="{5F318202-7931-4863-97A9-CC32D701A797}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
   <si>
     <t>Location</t>
   </si>
@@ -141,18 +141,6 @@
     <t>OR-1</t>
   </si>
   <si>
-    <t>OR-2</t>
-  </si>
-  <si>
-    <t>OR-3</t>
-  </si>
-  <si>
-    <t>OR-4</t>
-  </si>
-  <si>
-    <t>OR-5</t>
-  </si>
-  <si>
     <t>CO2-1</t>
   </si>
   <si>
@@ -177,16 +165,46 @@
     <t>ML195059</t>
   </si>
   <si>
+    <t>MJ190517</t>
+  </si>
+  <si>
+    <t>Boot Exchange</t>
+  </si>
+  <si>
+    <t>RTE 1</t>
+  </si>
+  <si>
+    <t>CPR3</t>
+  </si>
+  <si>
+    <t>CPR4</t>
+  </si>
+  <si>
+    <t>CPR5</t>
+  </si>
+  <si>
+    <t>CPR6</t>
+  </si>
+  <si>
+    <t>HF IQ</t>
+  </si>
+  <si>
+    <t>HF</t>
+  </si>
+  <si>
+    <t>MH183910</t>
+  </si>
+  <si>
+    <t>MI187991</t>
+  </si>
+  <si>
     <t>Oldie</t>
   </si>
   <si>
-    <t>MJ190517</t>
-  </si>
-  <si>
-    <t>Boot Exchange</t>
-  </si>
-  <si>
-    <t>RTE 1</t>
+    <t>HF23</t>
+  </si>
+  <si>
+    <t>IQ9</t>
   </si>
 </sst>
 </file>
@@ -545,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE12825-5FA0-48A1-B0CB-3F43941314C4}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,10 +587,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -631,7 +649,7 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -648,7 +666,7 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -670,7 +688,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -684,7 +702,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
@@ -698,7 +716,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -712,7 +730,7 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
@@ -782,10 +800,10 @@
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -796,10 +814,10 @@
         <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -809,7 +827,7 @@
       <c r="A18" t="s">
         <v>27</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C18" t="s">
@@ -820,22 +838,56 @@
       <c r="A19" t="s">
         <v>4</v>
       </c>
-      <c r="B19" t="s">
-        <v>47</v>
+      <c r="B19" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>48</v>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>